<commit_message>
Add guideline for Git
</commit_message>
<xml_diff>
--- a/Training-Plan-DevOps.xlsx
+++ b/Training-Plan-DevOps.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\devops-from-zero\lypt2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\devops-from-zero\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>TARGET DATE(S)</t>
   </si>
@@ -70,18 +70,7 @@
     <t>ISSUES</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>How to use Docker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic Linux
-1. Common command
-1. User, Group, Security
-2.  File, Folder, Devices
-3.  Networking: DHCP, DNS, SAMBA...
-</t>
   </si>
   <si>
     <t>Learn Elastic Load Balance (ELB)</t>
@@ -101,22 +90,7 @@
 2. CloudWatch</t>
   </si>
   <si>
-    <t>14/9/2019</t>
-  </si>
-  <si>
-    <t>20/11/2019</t>
-  </si>
-  <si>
-    <t>15/8/2019</t>
-  </si>
-  <si>
-    <t>19/8/2019</t>
-  </si>
-  <si>
     <t>21/8/2019</t>
-  </si>
-  <si>
-    <t>16/10/2019</t>
   </si>
   <si>
     <t>Learn  RDS, DynamoDB in AWS</t>
@@ -134,6 +108,33 @@
     <t>How to use Git Hub
 1. Command common
 2.  Manage branches ( merge, rebase)</t>
+  </si>
+  <si>
+    <t>1. Overview about git
+2. Create new repositories
+3. Command 
+4. Rebase and conflict</t>
+  </si>
+  <si>
+    <t>20/8/2019</t>
+  </si>
+  <si>
+    <t>22/9/2019</t>
+  </si>
+  <si>
+    <t>23/8/2019</t>
+  </si>
+  <si>
+    <t>26/10/2019</t>
+  </si>
+  <si>
+    <t>27/8/2019</t>
+  </si>
+  <si>
+    <t>28/11/2019</t>
+  </si>
+  <si>
+    <t>29/8/2019</t>
   </si>
   <si>
     <t>Learn command following:
@@ -141,9 +142,53 @@
 2. Device
 3. User &amp; Groups
 4. File &amp; Folder
-5. Compose 
-6. Filter
-7. Installation</t>
+5. Compose
+6. Filter content in file 
+7. Installation Nginx, Squid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Linux
+1. Common command
+1. User, Group, Security
+2.  File, Folder, Devices
+3.  Networking: Squid, Webmin, Nginx, Firewall...
+</t>
+  </si>
+  <si>
+    <t>1. How to install docker
+2. How to make image in docker</t>
+  </si>
+  <si>
+    <t>1. What is IAM in AWS?
+2. Why do we need use it?</t>
+  </si>
+  <si>
+    <t>1. What is S3 in AWS?
+2. Why do we need use it?</t>
+  </si>
+  <si>
+    <t>1. What is EC2 in AWS?
+2. Why do we need use it?</t>
+  </si>
+  <si>
+    <t>1. What is RDS, DynamoDB in AWS?
+2. Why do we need use it?</t>
+  </si>
+  <si>
+    <t>1. What is VPC in AWS?
+2. Why do we need use it?</t>
+  </si>
+  <si>
+    <t>1. What is ELB in AWS?
+2. Why do we need use it?</t>
+  </si>
+  <si>
+    <t>1. What is Route 53 DNS in AWS?
+2. Why do we need use it?</t>
+  </si>
+  <si>
+    <t>1. What is CloudTrail, CloudWatch in AWS?
+2. Why do we need use it?</t>
   </si>
 </sst>
 </file>
@@ -678,7 +723,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -744,8 +789,8 @@
       <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="16">
-        <v>43682</v>
+      <c r="C4" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="D4" s="19">
         <v>1</v>
@@ -753,54 +798,54 @@
       <c r="E4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>12</v>
-      </c>
+      <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="110.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="16">
-        <v>43683</v>
+        <v>33</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="D5" s="19">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>12</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C6" s="16">
-        <v>43683</v>
+        <v>43693</v>
       </c>
       <c r="D6" s="19">
-        <v>2</v>
-      </c>
-      <c r="E6" s="16"/>
+        <v>8</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="16">
-        <v>43684</v>
+        <v>43696</v>
       </c>
       <c r="D7" s="19">
-        <v>4</v>
-      </c>
-      <c r="E7" s="16"/>
+        <v>8</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
@@ -850,73 +895,83 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="16">
-        <v>43807</v>
+        <v>22</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>25</v>
       </c>
       <c r="D13" s="14">
         <v>3</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="22" t="s">
+        <v>35</v>
+      </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" s="15">
         <v>3</v>
       </c>
-      <c r="E14" s="16"/>
+      <c r="E14" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D15" s="14">
         <v>3</v>
       </c>
-      <c r="E15" s="16"/>
+      <c r="E15" s="22" t="s">
+        <v>37</v>
+      </c>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D16" s="14">
         <v>3</v>
       </c>
-      <c r="E16" s="16"/>
+      <c r="E16" s="22" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D17" s="15">
         <v>3</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="22" t="s">
+        <v>39</v>
+      </c>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
@@ -960,43 +1015,49 @@
     </row>
     <row r="22" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D22" s="14">
         <v>3</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="22" t="s">
+        <v>40</v>
+      </c>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
     <row r="23" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D23" s="15">
         <v>3</v>
       </c>
-      <c r="E23" s="16"/>
+      <c r="E23" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
     <row r="24" spans="2:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D24" s="14">
         <v>3</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="22" t="s">
+        <v>42</v>
+      </c>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>

</xml_diff>